<commit_message>
anpassen der tuple und records in Bezug auf leere Felder
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Spalte 1</t>
   </si>
@@ -34,21 +34,34 @@
     <t>Foo Widget</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
     <t>test2</t>
   </si>
   <si>
     <t>Bar Widget</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>Test5</t>
+  </si>
+  <si>
+    <t>test6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="&quot;WAHR&quot;;&quot;WAHR&quot;;&quot;FALSCH&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -115,8 +128,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -137,10 +154,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.6"/>
@@ -172,16 +189,54 @@
       <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>6</v>
+      <c r="D2" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>200</v>
+      </c>
+      <c r="D3" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D7" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>